<commit_message>
added hover on detail view
</commit_message>
<xml_diff>
--- a/new-variables-columns.xlsx
+++ b/new-variables-columns.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28780" windowHeight="16640" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18040" windowHeight="16480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="105">
   <si>
     <t>01TMEAN Trendline</t>
   </si>
@@ -156,9 +156,6 @@
     <t>Column Number</t>
   </si>
   <si>
-    <t>CSV Column Title</t>
-  </si>
-  <si>
     <t>Variable Name</t>
   </si>
   <si>
@@ -292,13 +289,58 @@
   </si>
   <si>
     <t>pge2</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>°C</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>Julian day</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Julian Day</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>days</t>
+  </si>
+  <si>
+    <t>CSV Index Title</t>
+  </si>
+  <si>
+    <t>NCOLOR</t>
+  </si>
+  <si>
+    <t>COLOR</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blue </t>
+  </si>
+  <si>
+    <t>green</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -344,6 +386,12 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -362,7 +410,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -402,14 +450,46 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="65">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -429,6 +509,19 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -448,6 +541,19 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -777,514 +883,922 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27.5" customWidth="1"/>
-    <col min="2" max="3" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1">
+    <row r="1" spans="1:6" s="3" customFormat="1">
       <c r="A1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2">
+        <v>46</v>
+      </c>
+      <c r="C2" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3">
+        <v>47</v>
+      </c>
+      <c r="C3" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4">
+        <v>48</v>
+      </c>
+      <c r="C4" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5">
+        <v>49</v>
+      </c>
+      <c r="C5" s="5">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6">
+        <v>50</v>
+      </c>
+      <c r="C6" s="5">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7">
+        <v>51</v>
+      </c>
+      <c r="C7" s="5">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8">
+        <v>52</v>
+      </c>
+      <c r="C8" s="5">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9">
+        <v>53</v>
+      </c>
+      <c r="C9" s="5">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10">
+        <v>54</v>
+      </c>
+      <c r="C10" s="5">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E10" t="s">
+        <v>101</v>
+      </c>
+      <c r="F10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11">
+        <v>55</v>
+      </c>
+      <c r="C11" s="5">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" t="s">
+        <v>102</v>
+      </c>
+      <c r="F11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12">
+        <v>56</v>
+      </c>
+      <c r="C12" s="5">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" t="s">
+        <v>102</v>
+      </c>
+      <c r="F12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13">
+        <v>57</v>
+      </c>
+      <c r="C13" s="5">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" t="s">
+        <v>102</v>
+      </c>
+      <c r="F13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14">
+        <v>58</v>
+      </c>
+      <c r="C14" s="5">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" t="s">
+        <v>102</v>
+      </c>
+      <c r="F14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15">
+        <v>59</v>
+      </c>
+      <c r="C15" s="5">
         <v>28</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" t="s">
+        <v>102</v>
+      </c>
+      <c r="F15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16">
+        <v>60</v>
+      </c>
+      <c r="C16" s="5">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" t="s">
+        <v>102</v>
+      </c>
+      <c r="F16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17">
+        <v>61</v>
+      </c>
+      <c r="C17" s="5">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E17" t="s">
+        <v>102</v>
+      </c>
+      <c r="F17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18">
+        <v>62</v>
+      </c>
+      <c r="C18" s="5">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18" t="s">
+        <v>94</v>
+      </c>
+      <c r="E18" t="s">
+        <v>101</v>
+      </c>
+      <c r="F18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19">
+        <v>63</v>
+      </c>
+      <c r="C19" s="5">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" t="s">
+        <v>101</v>
+      </c>
+      <c r="F19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20">
+        <v>64</v>
+      </c>
+      <c r="C20" s="5">
         <v>38</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" t="s">
+        <v>101</v>
+      </c>
+      <c r="F20" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
-      </c>
-      <c r="C21">
+        <v>65</v>
+      </c>
+      <c r="C21" s="5">
         <v>40</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" t="s">
+        <v>101</v>
+      </c>
+      <c r="F21" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22">
+        <v>66</v>
+      </c>
+      <c r="C22" s="5">
         <v>42</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22" t="s">
+        <v>101</v>
+      </c>
+      <c r="F22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23">
+        <v>67</v>
+      </c>
+      <c r="C23" s="5">
         <v>44</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="D23" t="s">
+        <v>94</v>
+      </c>
+      <c r="E23" t="s">
+        <v>101</v>
+      </c>
+      <c r="F23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
-      </c>
-      <c r="C24">
+        <v>68</v>
+      </c>
+      <c r="C24" s="5">
         <v>46</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="D24" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" t="s">
+        <v>101</v>
+      </c>
+      <c r="F24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
-      </c>
-      <c r="C25">
+        <v>69</v>
+      </c>
+      <c r="C25" s="5">
         <v>48</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="D25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E25" t="s">
+        <v>101</v>
+      </c>
+      <c r="F25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>71</v>
-      </c>
-      <c r="C26">
+        <v>70</v>
+      </c>
+      <c r="C26" s="5">
         <v>50</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="D26" t="s">
+        <v>92</v>
+      </c>
+      <c r="E26" t="s">
+        <v>102</v>
+      </c>
+      <c r="F26" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C27">
+        <v>71</v>
+      </c>
+      <c r="C27" s="5">
         <v>52</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="D27" t="s">
+        <v>95</v>
+      </c>
+      <c r="E27" t="s">
+        <v>102</v>
+      </c>
+      <c r="F27" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>73</v>
-      </c>
-      <c r="C28">
+        <v>72</v>
+      </c>
+      <c r="C28" s="5">
         <v>54</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="D28" t="s">
+        <v>95</v>
+      </c>
+      <c r="E28" t="s">
+        <v>102</v>
+      </c>
+      <c r="F28" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>74</v>
-      </c>
-      <c r="C29">
+        <v>73</v>
+      </c>
+      <c r="C29" s="5">
         <v>56</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="D29" t="s">
+        <v>91</v>
+      </c>
+      <c r="E29" t="s">
+        <v>102</v>
+      </c>
+      <c r="F29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>75</v>
-      </c>
-      <c r="C30">
+        <v>74</v>
+      </c>
+      <c r="C30" s="5">
         <v>58</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="D30" t="s">
+        <v>91</v>
+      </c>
+      <c r="E30" t="s">
+        <v>102</v>
+      </c>
+      <c r="F30" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>76</v>
-      </c>
-      <c r="C31">
+        <v>75</v>
+      </c>
+      <c r="C31" s="5">
         <v>60</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="D31" t="s">
+        <v>91</v>
+      </c>
+      <c r="E31" t="s">
+        <v>102</v>
+      </c>
+      <c r="F31" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>77</v>
-      </c>
-      <c r="C32">
+        <v>76</v>
+      </c>
+      <c r="C32" s="5">
         <v>62</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="D32" t="s">
+        <v>96</v>
+      </c>
+      <c r="E32" t="s">
+        <v>102</v>
+      </c>
+      <c r="F32" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
-      </c>
-      <c r="C33">
+        <v>77</v>
+      </c>
+      <c r="C33" s="5">
         <v>64</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
+      <c r="D33" t="s">
+        <v>96</v>
+      </c>
+      <c r="E33" t="s">
+        <v>102</v>
+      </c>
+      <c r="F33" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>79</v>
-      </c>
-      <c r="C34">
+        <v>78</v>
+      </c>
+      <c r="C34" s="5">
         <v>66</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
+      <c r="D34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E34" t="s">
+        <v>102</v>
+      </c>
+      <c r="F34" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>80</v>
-      </c>
-      <c r="C35">
+        <v>79</v>
+      </c>
+      <c r="C35" s="5">
         <v>68</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
+      <c r="D35" t="s">
+        <v>96</v>
+      </c>
+      <c r="E35" t="s">
+        <v>102</v>
+      </c>
+      <c r="F35" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>81</v>
-      </c>
-      <c r="C36">
+        <v>80</v>
+      </c>
+      <c r="C36" s="5">
         <v>70</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
+      <c r="D36" t="s">
+        <v>96</v>
+      </c>
+      <c r="E36" t="s">
+        <v>102</v>
+      </c>
+      <c r="F36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>90</v>
-      </c>
-      <c r="C37">
+        <v>89</v>
+      </c>
+      <c r="C37" s="5">
         <v>72</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="D37" t="s">
+        <v>92</v>
+      </c>
+      <c r="E37" t="s">
+        <v>102</v>
+      </c>
+      <c r="F37" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>82</v>
-      </c>
-      <c r="C38">
+        <v>81</v>
+      </c>
+      <c r="C38" s="5">
         <v>74</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
+      <c r="D38" t="s">
+        <v>92</v>
+      </c>
+      <c r="E38" t="s">
+        <v>102</v>
+      </c>
+      <c r="F38" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>83</v>
-      </c>
-      <c r="C39">
+        <v>82</v>
+      </c>
+      <c r="C39" s="5">
         <v>76</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
+      <c r="D39" t="s">
+        <v>92</v>
+      </c>
+      <c r="E39" t="s">
+        <v>102</v>
+      </c>
+      <c r="F39" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>84</v>
-      </c>
-      <c r="C40">
+        <v>83</v>
+      </c>
+      <c r="C40" s="5">
         <v>78</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
+      <c r="D40" t="s">
+        <v>96</v>
+      </c>
+      <c r="E40" t="s">
+        <v>102</v>
+      </c>
+      <c r="F40" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>85</v>
-      </c>
-      <c r="C41">
+        <v>84</v>
+      </c>
+      <c r="C41" s="5">
         <v>80</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
+      <c r="D41" t="s">
+        <v>96</v>
+      </c>
+      <c r="E41" t="s">
+        <v>102</v>
+      </c>
+      <c r="F41" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>86</v>
-      </c>
-      <c r="C42">
+        <v>85</v>
+      </c>
+      <c r="C42" s="5">
         <v>82</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
+      <c r="D42" t="s">
+        <v>96</v>
+      </c>
+      <c r="E42" t="s">
+        <v>102</v>
+      </c>
+      <c r="F42" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>87</v>
-      </c>
-      <c r="C43">
+        <v>86</v>
+      </c>
+      <c r="C43" s="5">
         <v>84</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
+      <c r="D43" t="s">
+        <v>94</v>
+      </c>
+      <c r="E43" t="s">
+        <v>102</v>
+      </c>
+      <c r="F43" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>88</v>
-      </c>
-      <c r="C44">
+        <v>87</v>
+      </c>
+      <c r="C44" s="5">
         <v>86</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="D44" t="s">
+        <v>97</v>
+      </c>
+      <c r="E44" t="s">
+        <v>101</v>
+      </c>
+      <c r="F44" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>89</v>
-      </c>
-      <c r="C45">
         <v>88</v>
       </c>
+      <c r="C45" s="5">
+        <v>88</v>
+      </c>
+      <c r="D45" t="s">
+        <v>97</v>
+      </c>
+      <c r="E45" t="s">
+        <v>102</v>
+      </c>
+      <c r="F45" t="s">
+        <v>101</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>